<commit_message>
Write range instead of write cell
</commit_message>
<xml_diff>
--- a/WikiPages.xlsx
+++ b/WikiPages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adyma\Documents\GitHub\APIs-GetLinksFromWiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1976326-A1A6-42AF-849C-4C4BC37740A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F02969-3CE1-4FB1-9770-9F98B0D2AFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="1995">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="1996">
   <x:si>
     <x:t>Wiki page name</x:t>
   </x:si>
@@ -45,6 +45,9 @@
   </x:si>
   <x:si>
     <x:t>Craig_Noone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Links</x:t>
   </x:si>
   <x:si>
     <x:t>Barbra Streisand</x:t>
@@ -6355,7 +6358,7 @@
   <x:dimension ref="A1:A5"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2"/>
+      <x:selection activeCell="A8" sqref="A8 A8:A8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6387,6 +6390,9 @@
       <x:c r="A5" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
+    </x:row>
+    <x:row r="8" spans="1:1">
+      <x:c r="A8" s="2" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -6402,7 +6408,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A1"/>
+  <x:dimension ref="A1:A45"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -6626,6 +6632,11 @@
     <x:row r="44" spans="1:1">
       <x:c r="A44" s="2" t="s">
         <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:1">
+      <x:c r="A45" s="2" t="s">
+        <x:v>49</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -6642,7 +6653,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A1"/>
+  <x:dimension ref="A1:A703"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -6650,7 +6661,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="2" t="s">
-        <x:v>49</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
@@ -10156,6 +10167,11 @@
     <x:row r="702" spans="1:1">
       <x:c r="A702" s="2" t="s">
         <x:v>750</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="703" spans="1:1">
+      <x:c r="A703" s="2" t="s">
+        <x:v>751</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -10172,7 +10188,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A1"/>
+  <x:dimension ref="A1:A1134"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -10180,7 +10196,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="2" t="s">
-        <x:v>751</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
@@ -10265,7 +10281,7 @@
     </x:row>
     <x:row r="18" spans="1:1">
       <x:c r="A18" s="2" t="s">
-        <x:v>372</x:v>
+        <x:v>768</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:1">
@@ -10275,7 +10291,7 @@
     </x:row>
     <x:row r="20" spans="1:1">
       <x:c r="A20" s="2" t="s">
-        <x:v>768</x:v>
+        <x:v>374</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:1">
@@ -12710,12 +12726,12 @@
     </x:row>
     <x:row r="507" spans="1:1">
       <x:c r="A507" s="2" t="s">
-        <x:v>32</x:v>
+        <x:v>1255</x:v>
       </x:c>
     </x:row>
     <x:row r="508" spans="1:1">
       <x:c r="A508" s="2" t="s">
-        <x:v>1255</x:v>
+        <x:v>33</x:v>
       </x:c>
     </x:row>
     <x:row r="509" spans="1:1">
@@ -13625,12 +13641,12 @@
     </x:row>
     <x:row r="690" spans="1:1">
       <x:c r="A690" s="2" t="s">
-        <x:v>46</x:v>
+        <x:v>1437</x:v>
       </x:c>
     </x:row>
     <x:row r="691" spans="1:1">
       <x:c r="A691" s="2" t="s">
-        <x:v>1437</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="692" spans="1:1">
@@ -14665,12 +14681,12 @@
     </x:row>
     <x:row r="898" spans="1:1">
       <x:c r="A898" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>1644</x:v>
       </x:c>
     </x:row>
     <x:row r="899" spans="1:1">
       <x:c r="A899" s="2" t="s">
-        <x:v>1644</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="900" spans="1:1">
@@ -14965,12 +14981,12 @@
     </x:row>
     <x:row r="958" spans="1:1">
       <x:c r="A958" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>1703</x:v>
       </x:c>
     </x:row>
     <x:row r="959" spans="1:1">
       <x:c r="A959" s="2" t="s">
-        <x:v>1703</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="960" spans="1:1">
@@ -15715,12 +15731,12 @@
     </x:row>
     <x:row r="1108" spans="1:1">
       <x:c r="A1108" s="2" t="s">
-        <x:v>48</x:v>
+        <x:v>1852</x:v>
       </x:c>
     </x:row>
     <x:row r="1109" spans="1:1">
       <x:c r="A1109" s="2" t="s">
-        <x:v>1852</x:v>
+        <x:v>49</x:v>
       </x:c>
     </x:row>
     <x:row r="1110" spans="1:1">
@@ -15841,6 +15857,11 @@
     <x:row r="1133" spans="1:1">
       <x:c r="A1133" s="2" t="s">
         <x:v>1876</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="1134" spans="1:1">
+      <x:c r="A1134" s="2" t="s">
+        <x:v>1877</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -15857,7 +15878,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A1"/>
+  <x:dimension ref="A1:A120"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -15865,7 +15886,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="2" t="s">
-        <x:v>1877</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
@@ -16165,12 +16186,12 @@
     </x:row>
     <x:row r="61" spans="1:1">
       <x:c r="A61" s="2" t="s">
-        <x:v>372</x:v>
+        <x:v>1937</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:1">
       <x:c r="A62" s="2" t="s">
-        <x:v>1937</x:v>
+        <x:v>373</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:1">
@@ -16456,6 +16477,11 @@
     <x:row r="119" spans="1:1">
       <x:c r="A119" s="2" t="s">
         <x:v>1994</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:1">
+      <x:c r="A120" s="2" t="s">
+        <x:v>1995</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>